<commit_message>
reminder:Appointment Follow-up Task and Referral Follow-up Task configuration
</commit_message>
<xml_diff>
--- a/config/forms/app/referral.xlsx
+++ b/config/forms/app/referral.xlsx
@@ -42,7 +42,7 @@
     <t>inputs</t>
   </si>
   <si>
-    <t>Viral Load test is due</t>
+    <t>NO_LABEL</t>
   </si>
   <si>
     <t>./source = 'user'</t>
@@ -57,9 +57,6 @@
     <t>source</t>
   </si>
   <si>
-    <t>NO_LABEL</t>
-  </si>
-  <si>
     <t>source_id</t>
   </si>
   <si>
@@ -120,7 +117,7 @@
     <t>reminder</t>
   </si>
   <si>
-    <t>select_one follow</t>
+    <t>select_one type</t>
   </si>
   <si>
     <t xml:space="preserve">Appointment Type
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>today()</t>
+  </si>
+  <si>
+    <t>select_one follow</t>
   </si>
   <si>
     <t>patient</t>
@@ -626,7 +626,7 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -646,7 +646,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
@@ -660,10 +660,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
@@ -677,10 +677,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -689,30 +689,30 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
@@ -723,13 +723,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
@@ -740,13 +740,13 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
@@ -757,13 +757,13 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
@@ -777,10 +777,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -792,10 +792,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -804,13 +804,13 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
@@ -821,13 +821,13 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
@@ -838,7 +838,7 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -849,7 +849,7 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -871,7 +871,7 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -882,35 +882,35 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="2"/>
     </row>
@@ -919,10 +919,10 @@
         <v>7</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="7" t="s">
@@ -952,54 +952,54 @@
     </row>
     <row r="22">
       <c r="A22" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="11" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>45</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="27">
       <c r="A27" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="C2" s="16" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-13_15-10</v>
+        <v>2022-07-18_16-46</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
auto:displaying data in the Referral Follow-up form  from the the appoitment schedule
</commit_message>
<xml_diff>
--- a/config/forms/app/referral.xlsx
+++ b/config/forms/app/referral.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
   <si>
     <t>type</t>
   </si>
@@ -60,6 +60,15 @@
     <t>source_id</t>
   </si>
   <si>
+    <t>my_field_referral</t>
+  </si>
+  <si>
+    <t>my_field_notes</t>
+  </si>
+  <si>
+    <t>my_field_date</t>
+  </si>
+  <si>
     <t>contact</t>
   </si>
   <si>
@@ -117,26 +126,26 @@
     <t>reminder</t>
   </si>
   <si>
-    <t>select_one type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appointment Type
+    <t>note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment Type : ${my_field_referral} referral
 </t>
   </si>
   <si>
     <t>note1</t>
   </si>
   <si>
-    <t>Any notes about this Appointment?</t>
+    <t xml:space="preserve">Any notes about this Appointment?:  ${my_field_notes} </t>
+  </si>
+  <si>
+    <t>when</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Appointment: ${my_field_date} </t>
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>when</t>
-  </si>
-  <si>
-    <t>Date of Appointment:</t>
   </si>
   <si>
     <t>date1</t>
@@ -175,18 +184,6 @@
   <si>
     <t xml:space="preserve">Keep this reminder in my Task List
 </t>
-  </si>
-  <si>
-    <t>type1</t>
-  </si>
-  <si>
-    <t>Internal Referral</t>
-  </si>
-  <si>
-    <t>type2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External Referral </t>
   </si>
   <si>
     <t>form_title</t>
@@ -312,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -330,6 +327,12 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -592,6 +595,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="20.0"/>
     <col customWidth="1" min="3" max="3" width="58.88"/>
     <col customWidth="1" min="5" max="5" width="22.25"/>
   </cols>
@@ -674,12 +678,12 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2"/>
@@ -688,79 +692,73 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1</v>
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
@@ -773,41 +771,45 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -820,197 +822,247 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1</v>
+      <c r="A14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>26</v>
+      <c r="A18" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8" t="s">
+      <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="11" t="s">
+      <c r="C23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="11" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="11" t="s">
+    </row>
+    <row r="26">
+      <c r="A26" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C26" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="11" t="s">
+    <row r="27">
+      <c r="A27" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C27" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F25" s="11" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="11" t="s">
+      <c r="B28" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="F28" s="13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="11" t="s">
-        <v>26</v>
+      <c r="G28" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1033,7 +1085,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1043,48 +1095,29 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>50</v>
+      <c r="A2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>52</v>
+      <c r="B3" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>56</v>
-      </c>
+      <c r="C4" s="14"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1106,47 +1139,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="14" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="17" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="18" t="str">
+        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
+        <v>2022-07-25_13-09</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="16" t="str">
-        <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-18_16-46</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto:removing today's date from viral and referral form
</commit_message>
<xml_diff>
--- a/config/forms/app/referral.xlsx
+++ b/config/forms/app/referral.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t>type</t>
   </si>
@@ -143,18 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">Date of Appointment: ${my_field_date} </t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>date1</t>
-  </si>
-  <si>
-    <t>Today’s Date</t>
-  </si>
-  <si>
-    <t>today()</t>
   </si>
   <si>
     <t>select_one follow</t>
@@ -1042,26 +1030,9 @@
       <c r="C28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="13" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1085,7 +1056,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1096,24 +1067,24 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -1139,47 +1110,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="18" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2022-07-25_13-09</v>
+        <v>2022-07-27_15-10</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F2" s="19"/>
       <c r="G2" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>